<commit_message>
change OB ticker to TEAD in input.xlsx
</commit_message>
<xml_diff>
--- a/data_script/input.xlsx
+++ b/data_script/input.xlsx
@@ -1767,7 +1767,7 @@
     <t>Outbrain Inc.</t>
   </si>
   <si>
-    <t>OB</t>
+    <t>TEAD</t>
   </si>
   <si>
     <t>OLD DOMINION FREIGHT LINE, INC.</t>
@@ -31403,7 +31403,7 @@
       <c r="A264" s="8" t="s">
         <v>581</v>
       </c>
-      <c r="B264" s="9" t="s">
+      <c r="B264" s="21" t="s">
         <v>582</v>
       </c>
       <c r="C264" s="9" t="s">
@@ -69651,7 +69651,7 @@
       <c r="A265" s="8" t="s">
         <v>581</v>
       </c>
-      <c r="B265" s="9" t="s">
+      <c r="B265" s="21" t="s">
         <v>582</v>
       </c>
       <c r="C265" s="9" t="s">

</xml_diff>